<commit_message>
File ready with real data
</commit_message>
<xml_diff>
--- a/Doc/LOAN_BST_TARGET.xlsx
+++ b/Doc/LOAN_BST_TARGET.xlsx
@@ -14,28 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>CTG 1</t>
-  </si>
-  <si>
-    <t>CTG 2</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Jashore Branch</t>
-  </si>
-  <si>
-    <t>Dhaka</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>AREA_CODE</t>
   </si>
@@ -68,13 +47,58 @@
   </si>
   <si>
     <t>BST_NAME</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Dhaka Area</t>
+  </si>
+  <si>
+    <t>Ashkona Branch</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Chattogram Area 1</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>Chandgaon Branch</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>Feni SME Branch</t>
+  </si>
+  <si>
+    <t>BS0728</t>
+  </si>
+  <si>
+    <t>Md. Shawkat Hossain</t>
+  </si>
+  <si>
+    <t>BS1251</t>
+  </si>
+  <si>
+    <t>Md. Jamshed Alam</t>
+  </si>
+  <si>
+    <t>BS0901</t>
+  </si>
+  <si>
+    <t>Mohammad Elias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +122,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,14 +136,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="65"/>
-        <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -144,21 +157,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -192,30 +190,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,8 +519,8 @@
   </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,127 +528,128 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="8" width="19.42578125" customWidth="1"/>
+    <col min="6" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6">
-        <v>1222</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6">
-        <v>200</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="6">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <v>100</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
-        <v>1290</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6">
-        <v>300</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
+        <v>200</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <v>2003</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6">
-        <v>400</v>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>50</v>
       </c>
       <c r="K4" s="1"/>
     </row>

</xml_diff>